<commit_message>
update báo cáo chi tiết theo công nợ
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Chi tiet theo doi tuong/WF0004 CT_ NXTon_DT_Quy cach.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Chi tiet theo doi tuong/WF0004 CT_ NXTon_DT_Quy cach.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANGTHITIEUMAI\Products\ASOFT_ERP81\10_DOCUMENT\13_DETAIL_DESIGN\2.PROJECTS\2015\0.ERP PROJECTS\02.Quan ly mat hang theo quy cach\ASOFT-WM\2015-11-05 Bao cao\08. Man hinh WF0004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOFT\201512\10_DOCUMENT\13_DETAIL_DESIGN\Chi tiet theo doi tuong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="19320" windowHeight="9990" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="19320" windowHeight="9990" tabRatio="615" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="Help" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Data Input'!$A$1:$Q$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Data Input'!$A$1:$S$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Func Spec'!$A$1:$J$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Help!$A$1:$K$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Input Check'!$A$1:$O$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Item Screen'!$A$1:$N$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Layout Screen'!$A$1:$J$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Item Screen'!$A$1:$P$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Layout Screen'!$A$1:$N$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Update History'!$A$1:$J$43</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -90,7 +90,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Người cập nhật tài liệu</t>
+          <t xml:space="preserve">Người tạo tài liệu
+</t>
         </r>
       </text>
     </comment>
@@ -298,6 +299,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Người tạo tài liệu
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -327,6 +342,30 @@
       </text>
     </comment>
     <comment ref="H2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ngày tạo tài liệu</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +428,7 @@
     <author>vinhphong</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -400,32 +439,6 @@
             <family val="2"/>
           </rPr>
           <t>Thứ tự Enter, Tab</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tên của item trên màn hình</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Caption của item trên màn hình</t>
         </r>
       </text>
     </comment>
@@ -438,11 +451,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tên của Field ở DB tương ứng với Item trên màn hình</t>
+          <t>Tên của item trên màn hình</t>
         </r>
       </text>
     </comment>
     <comment ref="F4" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Caption của item trên màn hình</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tên của Field ở DB tương ứng với Item trên màn hình</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -468,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="1" shapeId="0">
+    <comment ref="I4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -485,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="1" shapeId="0">
+    <comment ref="J4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -498,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="K4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -512,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="1" shapeId="0">
+    <comment ref="L4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -604,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="1" shapeId="0">
+    <comment ref="M4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -639,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0" shapeId="0">
+    <comment ref="N4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -655,7 +694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="1" shapeId="0">
+    <comment ref="O4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -927,7 +966,45 @@
     <author>Le Thi Thu Hien</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Người tạo tài liệu
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ngày tạo tài liệu</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -944,7 +1021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -959,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="J4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -977,7 +1054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="K4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -991,7 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1005,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N4" authorId="0" shapeId="0">
+    <comment ref="P4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1096,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P4" authorId="1" shapeId="0">
+    <comment ref="R4" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1105,7 +1182,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Người cập nhật tài liệu</t>
+          <t xml:space="preserve">Người tạo tài liệu
+</t>
         </r>
       </text>
     </comment>
@@ -1271,7 +1349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="166">
   <si>
     <t>Detail Design</t>
   </si>
@@ -1831,6 +1909,107 @@
       </rPr>
       <t>@SQL002</t>
     </r>
+  </si>
+  <si>
+    <t>Thị Phượng</t>
+  </si>
+  <si>
+    <t>Customize Hoàng Trần (CustomizeIndex =51) 
+ - Bổ sung mẫu báo cáo theo mã phân tích đối tượng (AR0725)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t>CustomizeIndex</t>
+  </si>
+  <si>
+    <t>Ver 2.0</t>
+  </si>
+  <si>
+    <t>Theo dõi vỏ</t>
+  </si>
+  <si>
+    <t>IsBottle</t>
+  </si>
+  <si>
+    <t>Textbox</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Phân tích theo đối tượng</t>
+  </si>
+  <si>
+    <t>Mã phân tích  5</t>
+  </si>
+  <si>
+    <t>O05ID</t>
+  </si>
+  <si>
+    <t>ComboBox</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>In báo cáo AR0725_HT</t>
+  </si>
+  <si>
+    <t>@SQL003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>AP0725</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(  
+   @DivisionID as nvarchar(50),     
+   @WareHouseID  as nvarchar(50),     
+   @FromObjectID  as nvarchar(50),
+   @ToObjectID as nvarchar(50),
+   @FromInventoryID as nvarchar(50),
+   @ToInventoryID as nvarchar(50),
+@IsBottle as tinyint,
+   @FromMonth as int,
+   @FromYear as int,
+   @ToMonth as int,
+   @ToYear as int,
+   @FromDate as Datetime,
+   @ToDate as Datetime,
+   @IsDate as tinyint,
+   @FromAna01ID nvarchar(50), @ToAna01ID nvarchar(50),
+   @FromAna02ID nvarchar(50), @ToAna02ID nvarchar(50),
+   @FromAna03ID nvarchar(50), @ToAna03ID nvarchar(50),
+   @FromAna04ID nvarchar(50), @ToAna04ID nvarchar(50),
+   @FromAna05ID nvarchar(50), @ToAna05ID nvarchar(50),
+   @FromAna06ID nvarchar(50), @ToAna06ID nvarchar(50),
+   @FromAna07ID nvarchar(50), @ToAna07ID nvarchar(50),
+   @FromAna08ID nvarchar(50), @ToAna08ID nvarchar(50),
+   @FromAna09ID nvarchar(50), @ToAna09ID nvarchar(50),
+   @FromAna10ID nvarchar(50), @ToAna10ID nvarchar(50),
+  @FromO05ID nvarchar(50), @ToO05ID nvarchar(50),
+)</t>
+    </r>
+  </si>
+  <si>
+    <t>Nếu @IsSpecificate = 1 , @IsBottle = 1 và ReportID = 'AR0725_HT' thì thực thi @SQL003</t>
+  </si>
+  <si>
+    <t>CustomizeIndex = 51</t>
   </si>
 </sst>
 </file>
@@ -2172,7 +2351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2388,6 +2567,56 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2400,13 +2629,13 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2508,6 +2737,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2523,16 +2757,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1800852</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>77068</xdr:rowOff>
+      <xdr:colOff>657852</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>134218</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2555,7 +2789,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1219200" y="714375"/>
+          <a:off x="76200" y="619125"/>
           <a:ext cx="4496427" cy="6220693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2563,6 +2797,125 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>42075</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4581524" y="628650"/>
+          <a:ext cx="4490251" cy="6076950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rounded Rectangular Callout 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315450" y="3876675"/>
+          <a:ext cx="942975" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -98106"/>
+            <a:gd name="adj2" fmla="val -179475"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Customize</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Hoàng Trần</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2858,7 +3211,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:J8"/>
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2874,10 +3227,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="115"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2899,11 +3252,13 @@
       <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="72"/>
+      <c r="J1" s="35" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -2925,7 +3280,9 @@
       <c r="I2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="72"/>
+      <c r="J2" s="35">
+        <v>42394</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="36" t="s">
@@ -2940,14 +3297,14 @@
       <c r="D4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
     </row>
     <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="37">
@@ -2964,28 +3321,36 @@
         <f>H1</f>
         <v>Tiểu Mai</v>
       </c>
-      <c r="E5" s="94" t="s">
+      <c r="E5" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-    </row>
-    <row r="6" spans="1:10" ht="11.25" x14ac:dyDescent="0.15">
-      <c r="A6" s="63">
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+    </row>
+    <row r="6" spans="1:10" s="97" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="94">
         <v>2</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="99"/>
+      <c r="B6" s="95">
+        <v>2</v>
+      </c>
+      <c r="C6" s="96">
+        <v>42394</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="117" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="119"/>
     </row>
     <row r="7" spans="1:10" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A7" s="63">
@@ -2994,12 +3359,12 @@
       <c r="B7" s="64"/>
       <c r="C7" s="65"/>
       <c r="D7" s="63"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="37">
@@ -3008,12 +3373,12 @@
       <c r="B8" s="38"/>
       <c r="C8" s="39"/>
       <c r="D8" s="37"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="37">
@@ -3022,12 +3387,12 @@
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
       <c r="D9" s="37"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="37">
@@ -3036,12 +3401,12 @@
       <c r="B10" s="40"/>
       <c r="C10" s="39"/>
       <c r="D10" s="37"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="113"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="37">
@@ -3050,12 +3415,12 @@
       <c r="B11" s="40"/>
       <c r="C11" s="39"/>
       <c r="D11" s="37"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="37">
@@ -3064,12 +3429,12 @@
       <c r="B12" s="40"/>
       <c r="C12" s="39"/>
       <c r="D12" s="37"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="113"/>
+      <c r="J12" s="113"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="37">
@@ -3078,12 +3443,12 @@
       <c r="B13" s="40"/>
       <c r="C13" s="39"/>
       <c r="D13" s="37"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="37">
@@ -3092,12 +3457,12 @@
       <c r="B14" s="40"/>
       <c r="C14" s="39"/>
       <c r="D14" s="37"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="37">
@@ -3106,12 +3471,12 @@
       <c r="B15" s="40"/>
       <c r="C15" s="39"/>
       <c r="D15" s="37"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="37">
@@ -3120,12 +3485,12 @@
       <c r="B16" s="40"/>
       <c r="C16" s="39"/>
       <c r="D16" s="37"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
+      <c r="J16" s="113"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="37">
@@ -3134,12 +3499,12 @@
       <c r="B17" s="40"/>
       <c r="C17" s="39"/>
       <c r="D17" s="37"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="37">
@@ -3148,12 +3513,12 @@
       <c r="B18" s="40"/>
       <c r="C18" s="39"/>
       <c r="D18" s="37"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="113"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="37">
@@ -3162,12 +3527,12 @@
       <c r="B19" s="40"/>
       <c r="C19" s="39"/>
       <c r="D19" s="37"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="37">
@@ -3176,12 +3541,12 @@
       <c r="B20" s="40"/>
       <c r="C20" s="39"/>
       <c r="D20" s="37"/>
-      <c r="E20" s="93"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="93"/>
-      <c r="J20" s="93"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="37">
@@ -3190,12 +3555,12 @@
       <c r="B21" s="40"/>
       <c r="C21" s="39"/>
       <c r="D21" s="37"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="37">
@@ -3204,12 +3569,12 @@
       <c r="B22" s="40"/>
       <c r="C22" s="39"/>
       <c r="D22" s="37"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="93"/>
-      <c r="J22" s="93"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="37">
@@ -3218,12 +3583,12 @@
       <c r="B23" s="40"/>
       <c r="C23" s="39"/>
       <c r="D23" s="37"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="93"/>
-      <c r="J23" s="93"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="37">
@@ -3232,12 +3597,12 @@
       <c r="B24" s="40"/>
       <c r="C24" s="39"/>
       <c r="D24" s="37"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="93"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="93"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="113"/>
+      <c r="I24" s="113"/>
+      <c r="J24" s="113"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="37">
@@ -3246,12 +3611,12 @@
       <c r="B25" s="40"/>
       <c r="C25" s="39"/>
       <c r="D25" s="37"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="113"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="113"/>
+      <c r="J25" s="113"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="37">
@@ -3260,12 +3625,12 @@
       <c r="B26" s="40"/>
       <c r="C26" s="39"/>
       <c r="D26" s="37"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="93"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="37">
@@ -3274,12 +3639,12 @@
       <c r="B27" s="40"/>
       <c r="C27" s="39"/>
       <c r="D27" s="37"/>
-      <c r="E27" s="93"/>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="37">
@@ -3288,12 +3653,12 @@
       <c r="B28" s="40"/>
       <c r="C28" s="39"/>
       <c r="D28" s="37"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="93"/>
-      <c r="J28" s="93"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="37">
@@ -3302,12 +3667,12 @@
       <c r="B29" s="40"/>
       <c r="C29" s="39"/>
       <c r="D29" s="37"/>
-      <c r="E29" s="93"/>
-      <c r="F29" s="93"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="113"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="113"/>
+      <c r="J29" s="113"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="37">
@@ -3316,12 +3681,12 @@
       <c r="B30" s="40"/>
       <c r="C30" s="39"/>
       <c r="D30" s="37"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
+      <c r="E30" s="113"/>
+      <c r="F30" s="113"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="113"/>
+      <c r="I30" s="113"/>
+      <c r="J30" s="113"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="37">
@@ -3330,12 +3695,12 @@
       <c r="B31" s="40"/>
       <c r="C31" s="39"/>
       <c r="D31" s="37"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="37">
@@ -3344,12 +3709,12 @@
       <c r="B32" s="40"/>
       <c r="C32" s="39"/>
       <c r="D32" s="37"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
+      <c r="G32" s="113"/>
+      <c r="H32" s="113"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="113"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="37">
@@ -3358,12 +3723,12 @@
       <c r="B33" s="40"/>
       <c r="C33" s="39"/>
       <c r="D33" s="37"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
+      <c r="E33" s="113"/>
+      <c r="F33" s="113"/>
+      <c r="G33" s="113"/>
+      <c r="H33" s="113"/>
+      <c r="I33" s="113"/>
+      <c r="J33" s="113"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="37">
@@ -3372,12 +3737,12 @@
       <c r="B34" s="40"/>
       <c r="C34" s="39"/>
       <c r="D34" s="37"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="37">
@@ -3386,12 +3751,12 @@
       <c r="B35" s="40"/>
       <c r="C35" s="39"/>
       <c r="D35" s="37"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="113"/>
+      <c r="I35" s="113"/>
+      <c r="J35" s="113"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="37">
@@ -3400,12 +3765,12 @@
       <c r="B36" s="40"/>
       <c r="C36" s="39"/>
       <c r="D36" s="37"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="113"/>
+      <c r="G36" s="113"/>
+      <c r="H36" s="113"/>
+      <c r="I36" s="113"/>
+      <c r="J36" s="113"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="37">
@@ -3414,12 +3779,12 @@
       <c r="B37" s="40"/>
       <c r="C37" s="39"/>
       <c r="D37" s="37"/>
-      <c r="E37" s="93"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="37">
@@ -3428,12 +3793,12 @@
       <c r="B38" s="40"/>
       <c r="C38" s="39"/>
       <c r="D38" s="37"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="93"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="93"/>
-      <c r="I38" s="93"/>
-      <c r="J38" s="93"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="37">
@@ -3442,12 +3807,12 @@
       <c r="B39" s="40"/>
       <c r="C39" s="39"/>
       <c r="D39" s="37"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="113"/>
+      <c r="G39" s="113"/>
+      <c r="H39" s="113"/>
+      <c r="I39" s="113"/>
+      <c r="J39" s="113"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="37">
@@ -3456,12 +3821,12 @@
       <c r="B40" s="40"/>
       <c r="C40" s="39"/>
       <c r="D40" s="37"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="93"/>
-      <c r="H40" s="93"/>
-      <c r="I40" s="93"/>
-      <c r="J40" s="93"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
+      <c r="G40" s="113"/>
+      <c r="H40" s="113"/>
+      <c r="I40" s="113"/>
+      <c r="J40" s="113"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="37">
@@ -3470,12 +3835,12 @@
       <c r="B41" s="40"/>
       <c r="C41" s="39"/>
       <c r="D41" s="37"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="93"/>
-      <c r="I41" s="93"/>
-      <c r="J41" s="93"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="113"/>
+      <c r="G41" s="113"/>
+      <c r="H41" s="113"/>
+      <c r="I41" s="113"/>
+      <c r="J41" s="113"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="37">
@@ -3484,12 +3849,12 @@
       <c r="B42" s="40"/>
       <c r="C42" s="39"/>
       <c r="D42" s="37"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="93"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+      <c r="G42" s="113"/>
+      <c r="H42" s="113"/>
+      <c r="I42" s="113"/>
+      <c r="J42" s="113"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="37">
@@ -3498,12 +3863,12 @@
       <c r="B43" s="40"/>
       <c r="C43" s="39"/>
       <c r="D43" s="37"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="113"/>
+      <c r="H43" s="113"/>
+      <c r="I43" s="113"/>
+      <c r="J43" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -3564,8 +3929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3576,15 +3941,18 @@
     <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="22" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" style="22" customWidth="1"/>
-    <col min="7" max="10" width="12.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="22" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="115"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -3609,11 +3977,13 @@
       <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="71"/>
+      <c r="J1" s="35" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -3638,23 +4008,25 @@
       <c r="I2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="72"/>
+      <c r="J2" s="35">
+        <v>42394</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="101" t="s">
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="102"/>
+      <c r="J4" s="122"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="41"/>
@@ -3665,10 +4037,10 @@
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
       <c r="H5" s="43"/>
-      <c r="I5" s="108" t="s">
+      <c r="I5" s="128" t="s">
         <v>141</v>
       </c>
-      <c r="J5" s="109"/>
+      <c r="J5" s="129"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="41"/>
@@ -3679,8 +4051,8 @@
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
       <c r="H6" s="44"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="131"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="41"/>
@@ -3691,8 +4063,8 @@
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
       <c r="H7" s="44"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="111"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="131"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="41"/>
@@ -3703,8 +4075,8 @@
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
       <c r="H8" s="44"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="111"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="131"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="41"/>
@@ -3715,8 +4087,8 @@
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
       <c r="H9" s="44"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="111"/>
+      <c r="I9" s="130"/>
+      <c r="J9" s="131"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="41"/>
@@ -3727,8 +4099,8 @@
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
       <c r="H10" s="44"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="111"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="131"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="41"/>
@@ -3739,8 +4111,8 @@
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
       <c r="H11" s="44"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="131"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="41"/>
@@ -3751,8 +4123,8 @@
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
       <c r="H12" s="44"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="111"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="131"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="41"/>
@@ -3763,8 +4135,8 @@
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
       <c r="H13" s="44"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="111"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="131"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="41"/>
@@ -3775,8 +4147,8 @@
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
       <c r="H14" s="44"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="113"/>
+      <c r="I14" s="132"/>
+      <c r="J14" s="133"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="41"/>
@@ -3787,10 +4159,10 @@
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
       <c r="H15" s="45"/>
-      <c r="I15" s="101" t="s">
+      <c r="I15" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="102"/>
+      <c r="J15" s="122"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="41"/>
@@ -3801,10 +4173,10 @@
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
       <c r="H16" s="44"/>
-      <c r="I16" s="104" t="s">
+      <c r="I16" s="124" t="s">
         <v>142</v>
       </c>
-      <c r="J16" s="105"/>
+      <c r="J16" s="125"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="41"/>
@@ -3815,8 +4187,8 @@
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
       <c r="H17" s="44"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="107"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="127"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="41"/>
@@ -3827,8 +4199,8 @@
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
       <c r="H18" s="44"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="107"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="127"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="41"/>
@@ -3839,8 +4211,8 @@
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
       <c r="H19" s="44"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="107"/>
+      <c r="I19" s="126"/>
+      <c r="J19" s="127"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="41"/>
@@ -3851,8 +4223,8 @@
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
       <c r="H20" s="44"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="107"/>
+      <c r="I20" s="126"/>
+      <c r="J20" s="127"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="41"/>
@@ -3863,8 +4235,8 @@
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
       <c r="H21" s="44"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="107"/>
+      <c r="I21" s="126"/>
+      <c r="J21" s="127"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="41"/>
@@ -3875,8 +4247,8 @@
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
       <c r="H22" s="44"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="107"/>
+      <c r="I22" s="126"/>
+      <c r="J22" s="127"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="41"/>
@@ -3887,8 +4259,8 @@
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
       <c r="H23" s="44"/>
-      <c r="I23" s="106"/>
-      <c r="J23" s="107"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="127"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="41"/>
@@ -3899,8 +4271,8 @@
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
       <c r="H24" s="44"/>
-      <c r="I24" s="106"/>
-      <c r="J24" s="107"/>
+      <c r="I24" s="126"/>
+      <c r="J24" s="127"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="41"/>
@@ -3911,8 +4283,8 @@
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
       <c r="H25" s="44"/>
-      <c r="I25" s="106"/>
-      <c r="J25" s="107"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="127"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="41"/>
@@ -3923,8 +4295,8 @@
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
       <c r="H26" s="44"/>
-      <c r="I26" s="106"/>
-      <c r="J26" s="107"/>
+      <c r="I26" s="126"/>
+      <c r="J26" s="127"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="41"/>
@@ -3935,8 +4307,8 @@
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
       <c r="H27" s="44"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="107"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="127"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="41"/>
@@ -3947,8 +4319,8 @@
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
       <c r="H28" s="44"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="107"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="127"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="41"/>
@@ -3959,8 +4331,8 @@
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
       <c r="H29" s="44"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="107"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="127"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="41"/>
@@ -3971,8 +4343,8 @@
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
       <c r="H30" s="44"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="107"/>
+      <c r="I30" s="126"/>
+      <c r="J30" s="127"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="41"/>
@@ -3983,8 +4355,8 @@
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
       <c r="H31" s="44"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="107"/>
+      <c r="I31" s="126"/>
+      <c r="J31" s="127"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="41"/>
@@ -3995,8 +4367,8 @@
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
       <c r="H32" s="44"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="107"/>
+      <c r="I32" s="126"/>
+      <c r="J32" s="127"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="41"/>
@@ -4007,8 +4379,8 @@
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
       <c r="H33" s="44"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="107"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="127"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="41"/>
@@ -4019,8 +4391,8 @@
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
       <c r="H34" s="44"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="107"/>
+      <c r="I34" s="126"/>
+      <c r="J34" s="127"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="41"/>
@@ -4031,8 +4403,8 @@
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
       <c r="H35" s="44"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="107"/>
+      <c r="I35" s="126"/>
+      <c r="J35" s="127"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="41"/>
@@ -4043,8 +4415,8 @@
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
       <c r="H36" s="44"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="107"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="127"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="41"/>
@@ -4055,8 +4427,8 @@
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
       <c r="H37" s="44"/>
-      <c r="I37" s="106"/>
-      <c r="J37" s="107"/>
+      <c r="I37" s="126"/>
+      <c r="J37" s="127"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="41"/>
@@ -4067,8 +4439,8 @@
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
       <c r="H38" s="44"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="107"/>
+      <c r="I38" s="126"/>
+      <c r="J38" s="127"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="41"/>
@@ -4079,8 +4451,8 @@
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
       <c r="H39" s="44"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="107"/>
+      <c r="I39" s="126"/>
+      <c r="J39" s="127"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="41"/>
@@ -4091,8 +4463,8 @@
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
       <c r="H40" s="44"/>
-      <c r="I40" s="106"/>
-      <c r="J40" s="107"/>
+      <c r="I40" s="126"/>
+      <c r="J40" s="127"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="41"/>
@@ -4103,8 +4475,8 @@
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
       <c r="H41" s="44"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="107"/>
+      <c r="I41" s="126"/>
+      <c r="J41" s="127"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="41"/>
@@ -4115,8 +4487,8 @@
       <c r="F42" s="42"/>
       <c r="G42" s="42"/>
       <c r="H42" s="44"/>
-      <c r="I42" s="106"/>
-      <c r="J42" s="107"/>
+      <c r="I42" s="126"/>
+      <c r="J42" s="127"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="41"/>
@@ -4127,8 +4499,8 @@
       <c r="F43" s="42"/>
       <c r="G43" s="42"/>
       <c r="H43" s="44"/>
-      <c r="I43" s="106"/>
-      <c r="J43" s="107"/>
+      <c r="I43" s="126"/>
+      <c r="J43" s="127"/>
     </row>
     <row r="44" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="41"/>
@@ -4139,8 +4511,8 @@
       <c r="F44" s="42"/>
       <c r="G44" s="42"/>
       <c r="H44" s="44"/>
-      <c r="I44" s="106"/>
-      <c r="J44" s="107"/>
+      <c r="I44" s="126"/>
+      <c r="J44" s="127"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4152,7 +4524,7 @@
     <mergeCell ref="I15:J15"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"Ta,Regular"&amp;10CONFIDENTIAL&amp;C&amp;"Tahoma,Regular"&amp;10&amp;P&amp;R&amp;"Tahoma,Regular"&amp;10© 2010 ASOFT JSC. All rights reserved.</oddFooter>
@@ -4165,710 +4537,831 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView view="pageBreakPreview" topLeftCell="F1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="23" customWidth="1"/>
-    <col min="8" max="9" width="6.7109375" style="23" customWidth="1"/>
-    <col min="10" max="11" width="7.7109375" style="23" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="23" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="23" customWidth="1"/>
-    <col min="14" max="14" width="33" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="22"/>
+    <col min="2" max="2" width="6.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="23" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="23" customWidth="1"/>
+    <col min="10" max="11" width="6.7109375" style="23" customWidth="1"/>
+    <col min="12" max="13" width="7.7109375" style="23" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="23" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="23" customWidth="1"/>
+    <col min="16" max="16" width="33" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="str">
+      <c r="G1" s="27" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="H1" s="134" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="115"/>
-      <c r="H1" s="116" t="str">
+      <c r="I1" s="135"/>
+      <c r="J1" s="136" t="str">
         <f>'Update History'!F1</f>
         <v>WF0004</v>
       </c>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="30" t="s">
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="28" t="str">
+      <c r="O1" s="28" t="str">
         <f>'Update History'!H1</f>
         <v>Tiểu Mai</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="P1" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="29" t="s">
+    <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27" t="str">
+      <c r="G2" s="27" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - WM</v>
       </c>
-      <c r="F2" s="114" t="s">
+      <c r="H2" s="134" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="115"/>
-      <c r="H2" s="116" t="str">
+      <c r="I2" s="135"/>
+      <c r="J2" s="136" t="str">
         <f>'Update History'!F2</f>
         <v>Nhập xuất tồn chi tiết theo đối tượng</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="137"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="28">
+      <c r="O2" s="28">
         <f>'Update History'!H2</f>
         <v>42317</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="P2" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="21" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="21" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="F4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="G4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="H4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="I4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="L4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="M4" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="N4" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="O4" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="P4" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+    <row r="5" spans="1:16" s="103" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="98">
         <v>1</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-    </row>
-    <row r="6" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
+      <c r="B5" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="98">
+        <v>51</v>
+      </c>
+      <c r="D5" s="98">
+        <v>1</v>
+      </c>
+      <c r="E5" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="100" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="100" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="101" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="101" t="s">
+        <v>155</v>
+      </c>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
+      <c r="P5" s="100"/>
+    </row>
+    <row r="6" spans="1:16" s="103" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="98">
         <v>2</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-    </row>
-    <row r="7" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
+      <c r="B6" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="98">
+        <v>51</v>
+      </c>
+      <c r="D6" s="104"/>
+      <c r="E6" s="105" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="106"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="108"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+    </row>
+    <row r="7" spans="1:16" s="103" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="98">
         <v>3</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="79"/>
-    </row>
-    <row r="8" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="98">
+        <v>51</v>
+      </c>
+      <c r="D7" s="98">
+        <v>2</v>
+      </c>
+      <c r="E7" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="106" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="106" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="101" t="s">
+        <v>159</v>
+      </c>
+      <c r="I7" s="94" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" s="107">
+        <v>50</v>
+      </c>
+      <c r="K7" s="107"/>
+      <c r="L7" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="108"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="106"/>
+    </row>
+    <row r="8" spans="1:16" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>4</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="79"/>
-    </row>
-    <row r="9" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="79"/>
+    </row>
+    <row r="9" spans="1:16" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>5</v>
       </c>
       <c r="B9" s="31"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="76"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="57"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="79"/>
-    </row>
-    <row r="10" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="57"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="79"/>
+    </row>
+    <row r="10" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>6</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="76"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-    </row>
-    <row r="11" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+    </row>
+    <row r="11" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>7</v>
       </c>
       <c r="B11" s="31"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="76"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-    </row>
-    <row r="12" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+    </row>
+    <row r="12" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>8</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="76"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-    </row>
-    <row r="13" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+    </row>
+    <row r="13" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="37"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-    </row>
-    <row r="14" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+    </row>
+    <row r="14" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="37"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-    </row>
-    <row r="15" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+    </row>
+    <row r="15" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="37"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-    </row>
-    <row r="16" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+    </row>
+    <row r="16" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="37"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-    </row>
-    <row r="17" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+    </row>
+    <row r="17" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="37"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-    </row>
-    <row r="18" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+    </row>
+    <row r="18" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="37"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-    </row>
-    <row r="19" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+    </row>
+    <row r="19" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-    </row>
-    <row r="20" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+    </row>
+    <row r="20" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
       <c r="G20" s="37"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-    </row>
-    <row r="21" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+    </row>
+    <row r="21" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-    </row>
-    <row r="22" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+    </row>
+    <row r="22" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="37"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-    </row>
-    <row r="23" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+    </row>
+    <row r="23" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="37"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-    </row>
-    <row r="24" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="57"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+    </row>
+    <row r="24" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="37"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-    </row>
-    <row r="25" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+    </row>
+    <row r="25" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="37"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-    </row>
-    <row r="26" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+    </row>
+    <row r="26" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="37"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
-    </row>
-    <row r="27" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+    </row>
+    <row r="27" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="37"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
-    </row>
-    <row r="28" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+    </row>
+    <row r="28" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="37"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-    </row>
-    <row r="29" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="57"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+    </row>
+    <row r="29" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="37"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-    </row>
-    <row r="30" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="57"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+    </row>
+    <row r="30" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="37"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-    </row>
-    <row r="31" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+    </row>
+    <row r="31" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="37"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-    </row>
-    <row r="32" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+    </row>
+    <row r="32" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="37"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
-    </row>
-    <row r="33" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="57"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
+    </row>
+    <row r="33" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="37"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-    </row>
-    <row r="34" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+    </row>
+    <row r="34" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="37"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
-    </row>
-    <row r="35" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="57"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="56"/>
+    </row>
+    <row r="35" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="37"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-    </row>
-    <row r="36" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="57"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+    </row>
+    <row r="36" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="37"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-    </row>
-    <row r="37" spans="1:14" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="57"/>
+      <c r="N36" s="37"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+    </row>
+    <row r="37" spans="1:16" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="37"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="57"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E37">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G37">
       <formula1>"Textbox,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid,Image,Link,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I37">
       <formula1>"Text, Number, DateTime, Boolean"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K37 J10:J37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L37 M6:M37">
       <formula1>"   ,l"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J9 F13:F37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H37 L5:L9">
       <formula1>"I,O,I/O"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H12">
       <formula1>"Caption,Textbox,DateTimePicker,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid, Image,Link,Form,Frame,Menu,MenuItem,Other"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E5"/>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
@@ -4877,7 +5370,7 @@
     <oddFooter>&amp;L&amp;"Ta,Regular"&amp;10CONFIDENTIAL&amp;C&amp;"Tahoma,Regular"&amp;10&amp;P&amp;R&amp;"Tahoma,Regular"&amp;10© 2010 ASOFT JSC. All rights reserved.</oddFooter>
   </headerFooter>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="14" max="53" man="1"/>
+    <brk id="16" max="53" man="1"/>
   </colBreaks>
   <legacyDrawing r:id="rId2"/>
   <legacyDrawingHF r:id="rId3"/>
@@ -4889,7 +5382,7 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4909,32 +5402,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="115"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="122" t="str">
+      <c r="D1" s="142" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="E1" s="122"/>
-      <c r="F1" s="123" t="s">
+      <c r="E1" s="142"/>
+      <c r="F1" s="143" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="119" t="str">
+      <c r="G1" s="143"/>
+      <c r="H1" s="139" t="str">
         <f>'Update History'!F1</f>
         <v>WF0004</v>
       </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="114" t="s">
+      <c r="I1" s="140"/>
+      <c r="J1" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="121"/>
-      <c r="L1" s="115"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="135"/>
       <c r="M1" s="48" t="str">
         <f>'Update History'!H1</f>
         <v>Tiểu Mai</v>
@@ -4945,30 +5438,30 @@
       <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="122" t="str">
+      <c r="D2" s="142" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - WM</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="123" t="s">
+      <c r="E2" s="142"/>
+      <c r="F2" s="143" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="119" t="str">
+      <c r="G2" s="143"/>
+      <c r="H2" s="139" t="str">
         <f>'Update History'!F2</f>
         <v>Nhập xuất tồn chi tiết theo đối tượng</v>
       </c>
-      <c r="I2" s="120"/>
-      <c r="J2" s="114" t="s">
+      <c r="I2" s="140"/>
+      <c r="J2" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="121"/>
-      <c r="L2" s="115"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="135"/>
       <c r="M2" s="48">
         <f>'Update History'!H2</f>
         <v>42317</v>
@@ -6020,393 +6513,442 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="23" customWidth="1"/>
-    <col min="10" max="10" width="13" style="23" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="23" customWidth="1"/>
-    <col min="12" max="16" width="14.140625" style="23" customWidth="1"/>
-    <col min="17" max="17" width="14" style="23" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" style="23" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="23" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="22" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="22"/>
+    <col min="2" max="2" width="7.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="23" customWidth="1"/>
+    <col min="12" max="12" width="13" style="23" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="23" customWidth="1"/>
+    <col min="14" max="18" width="14.140625" style="23" customWidth="1"/>
+    <col min="19" max="19" width="14" style="23" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" style="23" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" style="23" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="22" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="122" t="str">
+      <c r="G1" s="142" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="F1" s="122"/>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="142"/>
+      <c r="I1" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="50" t="str">
+      <c r="J1" s="50" t="str">
         <f>'Update History'!F1</f>
         <v>WF0004</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="48" t="str">
+      <c r="L1" s="48" t="str">
         <f>'Update History'!H1</f>
         <v>Tiểu Mai</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="N1" s="35" t="s">
+        <v>147</v>
+      </c>
       <c r="O1" s="80"/>
       <c r="P1" s="80"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-    </row>
-    <row r="2" spans="1:19" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="30" t="s">
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+    </row>
+    <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="122" t="str">
+      <c r="G2" s="142" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - WM</v>
       </c>
-      <c r="F2" s="122"/>
-      <c r="G2" s="62" t="s">
+      <c r="H2" s="142"/>
+      <c r="I2" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="50" t="str">
+      <c r="J2" s="50" t="str">
         <f>'Update History'!F2</f>
         <v>Nhập xuất tồn chi tiết theo đối tượng</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="48">
+      <c r="L2" s="48">
         <f>'Update History'!H2</f>
         <v>42317</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="N2" s="35">
+        <v>42394</v>
+      </c>
       <c r="O2" s="80"/>
       <c r="P2" s="80"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-    </row>
-    <row r="4" spans="1:19" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+    </row>
+    <row r="4" spans="1:21" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="93" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="E4" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="F4" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="G4" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="H4" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="78" t="s">
+      <c r="I4" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="78" t="s">
+      <c r="J4" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="101" t="s">
+      <c r="K4" s="121" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="78" t="s">
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="122"/>
+      <c r="O4" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="78" t="s">
+      <c r="P4" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="Q4" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="P4" s="78" t="s">
+      <c r="R4" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="78" t="s">
+      <c r="S4" s="78" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="32" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="32" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="87"/>
       <c r="B5" s="87"/>
-      <c r="C5" s="88"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="87"/>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="88"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="92" t="s">
+      <c r="H5" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="I5" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="J5" s="89" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="124" t="s">
+      <c r="K5" s="144" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
+      <c r="L5" s="145"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="146"/>
+      <c r="O5" s="90"/>
       <c r="P5" s="88"/>
       <c r="Q5" s="88"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-    </row>
-    <row r="6" spans="1:19" s="32" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+    </row>
+    <row r="6" spans="1:21" s="32" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="87"/>
       <c r="B6" s="87"/>
-      <c r="C6" s="88"/>
+      <c r="C6" s="87"/>
       <c r="D6" s="87"/>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="88"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="H6" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="G6" s="92" t="s">
+      <c r="I6" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="J6" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="I6" s="124" t="s">
+      <c r="K6" s="144" t="s">
         <v>144</v>
       </c>
-      <c r="J6" s="125"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
+      <c r="L6" s="145"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="90"/>
       <c r="P6" s="88"/>
       <c r="Q6" s="88"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-    </row>
-    <row r="7" spans="1:19" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="88"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="60"/>
+    </row>
+    <row r="7" spans="1:21" s="32" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
+      <c r="B7" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="87">
+        <v>51</v>
+      </c>
       <c r="D7" s="87"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="92" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="K7" s="144" t="s">
+        <v>163</v>
+      </c>
+      <c r="L7" s="145"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="90"/>
       <c r="P7" s="88"/>
       <c r="Q7" s="88"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-    </row>
-    <row r="8" spans="1:19" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="60"/>
+    </row>
+    <row r="8" spans="1:21" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="87"/>
       <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="87"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="88"/>
       <c r="I8" s="88"/>
-      <c r="J8" s="88"/>
+      <c r="J8" s="89"/>
       <c r="K8" s="88"/>
       <c r="L8" s="88"/>
-      <c r="M8" s="90"/>
+      <c r="M8" s="88"/>
       <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
+      <c r="O8" s="90"/>
       <c r="P8" s="88"/>
       <c r="Q8" s="88"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-    </row>
-    <row r="9" spans="1:19" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+    </row>
+    <row r="9" spans="1:21" s="32" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="37"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="59"/>
       <c r="I9" s="59"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="74"/>
       <c r="N9" s="77"/>
       <c r="O9" s="77"/>
       <c r="P9" s="77"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="60"/>
-    </row>
-    <row r="10" spans="1:19" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="60"/>
+    </row>
+    <row r="10" spans="1:21" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
       <c r="G10" s="59"/>
       <c r="H10" s="59"/>
       <c r="I10" s="59"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="74"/>
       <c r="N10" s="77"/>
       <c r="O10" s="77"/>
       <c r="P10" s="77"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-    </row>
-    <row r="11" spans="1:19" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="60"/>
+    </row>
+    <row r="11" spans="1:21" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
       <c r="I11" s="59"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="74"/>
       <c r="N11" s="77"/>
       <c r="O11" s="77"/>
       <c r="P11" s="77"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-    </row>
-    <row r="12" spans="1:19" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="60"/>
+    </row>
+    <row r="12" spans="1:21" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="59"/>
       <c r="F12" s="59"/>
       <c r="G12" s="59"/>
       <c r="H12" s="59"/>
       <c r="I12" s="59"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
       <c r="N12" s="77"/>
       <c r="O12" s="77"/>
       <c r="P12" s="77"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="60"/>
-      <c r="S12" s="60"/>
-    </row>
-    <row r="13" spans="1:19" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
+      <c r="Q12" s="77"/>
+      <c r="R12" s="77"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="60"/>
+    </row>
+    <row r="13" spans="1:21" s="32" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="75"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
       <c r="G13" s="59"/>
       <c r="H13" s="59"/>
       <c r="I13" s="59"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="61"/>
       <c r="N13" s="77"/>
       <c r="O13" s="77"/>
       <c r="P13" s="77"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="77"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
+  <mergeCells count="7">
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K5:N5"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E13">
       <formula1>"Select,Insert,Delete,Update"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G6 D9:D13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I7 F9:F13">
       <formula1>"SQL Script, ID SQL, ID Store, ID Function, ID Trigger"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H7">
       <formula1>"Select,Insert,Update,Delete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5">
       <formula1>"Load,Click,Double Click,Change,Selected,KeyDown,KeyPress,Hover,Focus,LostFocus"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="O5"/>
+    <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q5"/>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
-  <pageSetup paperSize="9" scale="98" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"Ta,Regular"&amp;10CONFIDENTIAL&amp;C&amp;"Tahoma,Regular"&amp;10&amp;P&amp;R&amp;"Tahoma,Regular"&amp;10© 2010 ASOFT JSC. All rights reserved.</oddFooter>
@@ -6421,12 +6963,12 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="22" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="22" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="22" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="22" customWidth="1"/>
@@ -6437,10 +6979,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="115"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6465,11 +7007,13 @@
       <c r="I1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="35"/>
+      <c r="J1" s="35" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -6494,7 +7038,9 @@
       <c r="I2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="35">
+        <v>42394</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="81" t="s">
@@ -6786,28 +7332,35 @@
       <c r="I26" s="42"/>
       <c r="J26" s="45"/>
     </row>
-    <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="45"/>
-    </row>
-    <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="45"/>
+    <row r="27" spans="1:10" s="97" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="97" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="97" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="110"/>
+    </row>
+    <row r="28" spans="1:10" s="97" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="111"/>
+      <c r="B28" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="112"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="110"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="41"/>
@@ -7004,7 +7557,7 @@
   <dimension ref="B1:G62"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A49" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M76" sqref="M75:M76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7016,14 +7569,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
@@ -7216,11 +7769,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="128" t="s">
+      <c r="E27" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="129"/>
-      <c r="G27" s="130"/>
+      <c r="F27" s="149"/>
+      <c r="G27" s="150"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">

</xml_diff>

<commit_message>
chỉnh sửa một số sai xót trong nội dung
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Chi tiet theo doi tuong/WF0004 CT_ NXTon_DT_Quy cach.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Chi tiet theo doi tuong/WF0004 CT_ NXTon_DT_Quy cach.xlsx
@@ -2006,10 +2006,10 @@
     </r>
   </si>
   <si>
-    <t>Nếu @IsSpecificate = 1 , @IsBottle = 1 và ReportID = 'AR0725_HT' thì thực thi @SQL003</t>
-  </si>
-  <si>
     <t>CustomizeIndex = 51</t>
+  </si>
+  <si>
+    <t>Nếu  @IsBottle = 1 và ReportID = 'AR0725_HT' thì thực thi @SQL003</t>
   </si>
 </sst>
 </file>
@@ -3872,15 +3872,23 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="E26:J26"/>
@@ -3896,23 +3904,15 @@
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6963,7 +6963,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7337,7 +7337,7 @@
         <v>151</v>
       </c>
       <c r="B27" s="97" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="109"/>
       <c r="D27" s="109"/>
@@ -7351,7 +7351,7 @@
     <row r="28" spans="1:10" s="97" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="111"/>
       <c r="B28" s="109" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C28" s="112"/>
       <c r="D28" s="109"/>

</xml_diff>